<commit_message>
191113 Night Update 01
</commit_message>
<xml_diff>
--- a/Thesis/VAC Thesis 1.0/Chapter-4/tables/AcceleratedCorrosion_db075.xlsx
+++ b/Thesis/VAC Thesis 1.0/Chapter-4/tables/AcceleratedCorrosion_db075.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Condition-Dependent-PBEE\Thesis\VAC Thesis 1.0\Chapter-4\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC2F14F-6C03-430C-A485-05A129928FA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A35825-910F-404F-9BCB-EB16B8FA92F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -447,7 +447,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -564,19 +564,19 @@
         <v>1.1187151061949441</v>
       </c>
       <c r="C10">
-        <v>6.0000000000000001E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D10">
         <f>+C10*1000000/$B$7</f>
-        <v>56.386435468285285</v>
+        <v>46.988696223571068</v>
       </c>
       <c r="E10">
         <f>+(B10*$B$4*$B$3)/(C10*$B$2*60*60)</f>
-        <v>179.11062495224209</v>
+        <v>214.93274994269055</v>
       </c>
       <c r="F10">
         <f>+E10/24</f>
-        <v>7.4629427063434202</v>
+        <v>8.9555312476121056</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -589,19 +589,19 @@
       </c>
       <c r="C11">
         <f>+C10</f>
-        <v>6.0000000000000001E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D11">
         <f t="shared" ref="D11:D14" si="1">+C11*1000000/$B$7</f>
-        <v>56.386435468285285</v>
+        <v>46.988696223571068</v>
       </c>
       <c r="E11">
         <f t="shared" ref="E11:E14" si="2">+(B11*$B$4*$B$3)/(C11*$B$2*60*60)</f>
-        <v>358.22124990448418</v>
+        <v>429.8654998853811</v>
       </c>
       <c r="F11">
         <f t="shared" ref="F11:F14" si="3">+E11/24</f>
-        <v>14.92588541268684</v>
+        <v>17.911062495224211</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -614,19 +614,19 @@
       </c>
       <c r="C12">
         <f t="shared" ref="C12:C14" si="4">+C11</f>
-        <v>6.0000000000000001E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D12">
         <f t="shared" si="1"/>
-        <v>56.386435468285285</v>
+        <v>46.988696223571068</v>
       </c>
       <c r="E12">
         <f t="shared" si="2"/>
-        <v>537.33187485672636</v>
+        <v>644.79824982807168</v>
       </c>
       <c r="F12">
         <f t="shared" si="3"/>
-        <v>22.388828119030265</v>
+        <v>26.866593742836319</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -639,19 +639,19 @@
       </c>
       <c r="C13">
         <f t="shared" si="4"/>
-        <v>6.0000000000000001E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D13">
         <f t="shared" si="1"/>
-        <v>56.386435468285285</v>
+        <v>46.988696223571068</v>
       </c>
       <c r="E13">
         <f t="shared" si="2"/>
-        <v>716.44249980896836</v>
+        <v>859.7309997707622</v>
       </c>
       <c r="F13">
         <f t="shared" si="3"/>
-        <v>29.851770825373681</v>
+        <v>35.822124990448422</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -664,19 +664,19 @@
       </c>
       <c r="C14">
         <f t="shared" si="4"/>
-        <v>6.0000000000000001E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D14">
         <f t="shared" si="1"/>
-        <v>56.386435468285285</v>
+        <v>46.988696223571068</v>
       </c>
       <c r="E14">
         <f t="shared" si="2"/>
-        <v>895.5531247612106</v>
+        <v>1074.6637497134527</v>
       </c>
       <c r="F14">
         <f t="shared" si="3"/>
-        <v>37.314713531717111</v>
+        <v>44.77765623806053</v>
       </c>
     </row>
   </sheetData>

</xml_diff>